<commit_message>
Finished LME models for new metagenomic dataset
I finished running linear mixed effect models for the new metagenomic dataset and created a new copy of the Excel file "Linear mixed models, Cohen's D for main effects" with another tab for the new metagenomic dataset. Now, I'm beginning to run Tukey's post-hoc on the linear mixed effect model results.
</commit_message>
<xml_diff>
--- a/Statistical analyses/Linear mixed models, Cohen's D for main effects.xlsx
+++ b/Statistical analyses/Linear mixed models, Cohen's D for main effects.xlsx
@@ -10,13 +10,14 @@
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
     <sheet name="Vmax" sheetId="2" r:id="rId2"/>
     <sheet name="litterChem" sheetId="3" r:id="rId3"/>
+    <sheet name="CAZyme metagenomic" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>Note</t>
   </si>
@@ -66,6 +67,24 @@
     <t>significance level down to 0.05 later.</t>
   </si>
   <si>
+    <t>Ashish had also re-worked his metagenomic dataset to sum up the</t>
+  </si>
+  <si>
+    <t>number of CAZyme genes dedicated to a specific substrate per million</t>
+  </si>
+  <si>
+    <t>reads, as opposed to last time in which he calculated a proportion</t>
+  </si>
+  <si>
+    <t>of CAZyme genes dedicated to a specific substrate out of all</t>
+  </si>
+  <si>
+    <t>possible CAZyme genes. I analyzed this dataset using linear mixed</t>
+  </si>
+  <si>
+    <t>effect models as well.</t>
+  </si>
+  <si>
     <t>dependent</t>
   </si>
   <si>
@@ -142,6 +161,33 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>cellulose</t>
+  </si>
+  <si>
+    <t>chitin</t>
+  </si>
+  <si>
+    <t>hemicellulose</t>
+  </si>
+  <si>
+    <t>lignin</t>
+  </si>
+  <si>
+    <t>oligosaccharides</t>
+  </si>
+  <si>
+    <t>peptidoglycan</t>
+  </si>
+  <si>
+    <t>polysaccharides</t>
+  </si>
+  <si>
+    <t>starch</t>
+  </si>
+  <si>
+    <t>***</t>
   </si>
 </sst>
 </file>
@@ -499,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -583,6 +629,36 @@
     <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -600,35 +676,35 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>0.386959212373011</v>
@@ -636,10 +712,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>1.621452167886074</v>
@@ -650,18 +726,18 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>2.932820101780986</v>
@@ -672,10 +748,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>0.8143638474304012</v>
@@ -683,10 +759,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>2.499390463795144</v>
@@ -694,13 +770,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -718,35 +794,35 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>2.718168316076161</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>2.010863824245935</v>
@@ -754,10 +830,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>2.093819908757187</v>
@@ -765,7 +841,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>3.480164653078523</v>
@@ -773,10 +849,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
       </c>
       <c r="C6">
         <v>2.024099207391656</v>
@@ -784,23 +860,23 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>1.261016078762071</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>0.306570272488</v>
@@ -809,7 +885,110 @@
         <v>0.9758736643866422</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>0.1487382805060204</v>
+      </c>
+      <c r="D2">
+        <v>0.1136010621013912</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>0.8149801989992265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>1.657287342449503</v>
+      </c>
+      <c r="D4">
+        <v>0.310960681005965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>1.055639854891317</v>
+      </c>
+      <c r="D5">
+        <v>0.7646898136555431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>1.133114552810442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <v>1.333409736892981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>